<commit_message>
Added cost for a sun sensor
</commit_message>
<xml_diff>
--- a/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
+++ b/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Sun Sensor</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>too large</t>
+  </si>
+  <si>
+    <t>€ 4,890.00/unit (via cubesatshop)</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,8 +770,8 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>25</v>
+      <c r="G3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Made slides for sun sensors and Attitude Determination requirements, Added another possible sun sensor candidate
</commit_message>
<xml_diff>
--- a/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
+++ b/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Sun Sensor</t>
   </si>
@@ -90,9 +90,6 @@
     <t>http://www.solar-mems.com/smt_pdf/commercial_brochure_SSOC-A.pdf</t>
   </si>
   <si>
-    <t>SOLARMEMS SSoC-A</t>
-  </si>
-  <si>
     <t>unknown</t>
   </si>
   <si>
@@ -211,6 +208,33 @@
   </si>
   <si>
     <t>€ 4,890.00/unit (via cubesatshop)</t>
+  </si>
+  <si>
+    <t>SOLARMEMS SSoC-A60</t>
+  </si>
+  <si>
+    <t>SOLARMEMS nanoSSoC-D60</t>
+  </si>
+  <si>
+    <t>http://www.solar-mems.com/smt_pdf/Brochure_NanoSSOC-D60.pdf</t>
+  </si>
+  <si>
+    <t>&lt;23mA(?)</t>
+  </si>
+  <si>
+    <t>6.5 grams</t>
+  </si>
+  <si>
+    <t>&lt;0.5 deg</t>
+  </si>
+  <si>
+    <t>-30C to +85C</t>
+  </si>
+  <si>
+    <t>43x14x5.9mm</t>
+  </si>
+  <si>
+    <t>Try ADCOLE again since they're stuff is very good. If we run into a problem with sun sensors not being able to update fast enough, they may be able to help. Otherwise, maybe we'll have to do an intertial solution.</t>
   </si>
 </sst>
 </file>
@@ -325,7 +349,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -343,6 +367,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -649,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,13 +699,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -710,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,7 +752,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -756,40 +781,40 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="L3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
         <v>62</v>
-      </c>
-      <c r="M3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -797,156 +822,194 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="L5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="M5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="L7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" t="s">
         <v>60</v>
-      </c>
-      <c r="M7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heard back from some suppliers, added info
</commit_message>
<xml_diff>
--- a/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
+++ b/Documents/CubeSat_Sub-Systems/Atittude Control/Sun Sensor research.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>Sun Sensor</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Operating Temp</t>
   </si>
   <si>
-    <t>-25C to +50C</t>
-  </si>
-  <si>
     <t>114 deg.</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Color coding</t>
   </si>
   <si>
-    <t>I'm going to be making more calls this week to fill in the yellow</t>
-  </si>
-  <si>
     <t>36 grams</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>too large</t>
   </si>
   <si>
-    <t>€ 4,890.00/unit (via cubesatshop)</t>
-  </si>
-  <si>
     <t>SOLARMEMS SSoC-A60</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>http://www.solar-mems.com/smt_pdf/Brochure_NanoSSOC-D60.pdf</t>
   </si>
   <si>
-    <t>&lt;23mA(?)</t>
-  </si>
-  <si>
     <t>6.5 grams</t>
   </si>
   <si>
@@ -235,6 +223,30 @@
   </si>
   <si>
     <t>Try ADCOLE again since they're stuff is very good. If we run into a problem with sun sensors not being able to update fast enough, they may be able to help. Otherwise, maybe we'll have to do an intertial solution.</t>
+  </si>
+  <si>
+    <t>-25C to +50C (tested, components are rated for -40C to +85C)</t>
+  </si>
+  <si>
+    <t>Analog, requires ADC</t>
+  </si>
+  <si>
+    <t>50Hz (max 10Hz, if using I2C(?))</t>
+  </si>
+  <si>
+    <t>€ 3,600.00/unit</t>
+  </si>
+  <si>
+    <t>€ 2200.00/unit (via cubesatshop)</t>
+  </si>
+  <si>
+    <t>CEPHEUS and five confidential missions from Clyde Space and Innovative Space Solutions</t>
+  </si>
+  <si>
+    <t>115mW</t>
+  </si>
+  <si>
+    <t>No Reply</t>
   </si>
 </sst>
 </file>
@@ -317,27 +329,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -349,15 +346,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -368,6 +363,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -677,7 +673,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,13 +695,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -732,10 +728,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -743,37 +739,37 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -781,235 +777,233 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>23</v>
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="L5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
-        <v>42</v>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="4" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>49</v>
       </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C8" t="s">
+      <c r="J8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1020,6 +1014,7 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
     <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>